<commit_message>
intermediate revision - refactoring, part 1
</commit_message>
<xml_diff>
--- a/testng-dataproviders/data_2007.xlsx
+++ b/testng-dataproviders/data_2007.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,25 +22,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>SEARCH</t>
-  </si>
-  <si>
-    <t>COUNT</t>
-  </si>
-  <si>
-    <t>junit</t>
-  </si>
-  <si>
-    <t>testng</t>
-  </si>
-  <si>
-    <t>spock</t>
-  </si>
-  <si>
-    <t>there is no such thing</t>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEARCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">junit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no such thing</t>
   </si>
 </sst>
 </file>
@@ -48,7 +48,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,8 +115,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,63 +144,66 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>100</v>
+      <c r="C2" s="1" t="n">
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>40</v>
+      <c r="C3" s="1" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>10</v>
+      <c r="C4" s="1" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>